<commit_message>
Deploying to gh-pages from @ NIH-NCPI/ncpi-fhir-ig@322fe282ac235068eb6fd20329942bc487f958df 🚀
</commit_message>
<xml_diff>
--- a/CodeSystem-hpo.xlsx
+++ b/CodeSystem-hpo.xlsx
@@ -62,7 +62,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2022-10-11T14:47:05+00:00</t>
+    <t>2022-10-31T22:46:37+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -113,7 +113,7 @@
     <t>Content</t>
   </si>
   <si>
-    <t>complete</t>
+    <t>fragment</t>
   </si>
   <si>
     <t>Supplements</t>

</xml_diff>